<commit_message>
More work on Excel Manager Prototype
-Write functions can now handle String Based Addresses (A,1) instead of Index Based Address (0,0)
</commit_message>
<xml_diff>
--- a/Project Files/Excel Manage Prototype/Test.xlsx
+++ b/Project Files/Excel Manage Prototype/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CBNHS System\Project Files\Excel Manage Prototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98604445-8C3B-489F-9C5F-736DCF941419}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE6F932-FB85-4C6E-8891-DE2F221E32D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{9DAA83F0-7D37-4DC0-8154-5EE00742C550}"/>
   </bookViews>
@@ -25,17 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Yeet</t>
-  </si>
-  <si>
-    <t>Yo</t>
-  </si>
-  <si>
-    <t>Reee</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -385,26 +375,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A057ED4F-C60D-4A7F-A939-E81120426F1F}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made removing row functions
</commit_message>
<xml_diff>
--- a/Project Files/Excel Manage Prototype/Test.xlsx
+++ b/Project Files/Excel Manage Prototype/Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CBNHS System\Project Files\Excel Manage Prototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE6F932-FB85-4C6E-8891-DE2F221E32D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8373AB43-3BBB-47DE-815B-72B408629C4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{9DAA83F0-7D37-4DC0-8154-5EE00742C550}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15120" xr2:uid="{9DAA83F0-7D37-4DC0-8154-5EE00742C550}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+  <si>
+    <t>yYow</t>
+  </si>
+  <si>
+    <t>asdasd</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>asda</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>Dasdas</t>
+  </si>
+  <si>
+    <t>asdas</t>
+  </si>
+  <si>
+    <t>agasfags</t>
+  </si>
+  <si>
+    <t>dfefgxg</t>
+  </si>
+  <si>
+    <t>sfdsghs</t>
+  </si>
+  <si>
+    <t>sfsdf</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -375,14 +409,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A057ED4F-C60D-4A7F-A939-E81120426F1F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Recovered Registration System from data corruption
-
</commit_message>
<xml_diff>
--- a/Project Files/Excel Manage Prototype/Test.xlsx
+++ b/Project Files/Excel Manage Prototype/Test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CBNHS System\Project Files\Excel Manage Prototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8373AB43-3BBB-47DE-815B-72B408629C4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691677CE-C477-4DDE-9C08-E5A461FDFC5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15120" xr2:uid="{9DAA83F0-7D37-4DC0-8154-5EE00742C550}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>yYow</t>
   </si>
@@ -58,6 +58,21 @@
   </si>
   <si>
     <t>sfsdf</t>
+  </si>
+  <si>
+    <t>last1</t>
+  </si>
+  <si>
+    <t>last2</t>
+  </si>
+  <si>
+    <t>last3</t>
+  </si>
+  <si>
+    <t>last4</t>
+  </si>
+  <si>
+    <t>last5</t>
   </si>
 </sst>
 </file>
@@ -409,23 +424,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A057ED4F-C60D-4A7F-A939-E81120426F1F}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -441,8 +459,11 @@
       <c r="E2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -455,10 +476,13 @@
       <c r="E3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <v>12524734</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -472,33 +496,42 @@
       <c r="E4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="Q6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>

</xml_diff>